<commit_message>
update file excel usa
</commit_message>
<xml_diff>
--- a/01_data_clean/macro/UNRATE_USA.xlsx
+++ b/01_data_clean/macro/UNRATE_USA.xlsx
@@ -5,49 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaia\Documents\magistrale\AMUniversite\credit risk\DRIM2025_Project0\01_data_clean\macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8610441A-909D-48FE-A4B7-C8F5333CA5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3969D9E0-90DF-490D-B523-4703588D93EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="README" sheetId="1" r:id="rId1"/>
-    <sheet name="Monthly" sheetId="2" r:id="rId2"/>
+    <sheet name="Monthly" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>FRED Graph Observations</t>
-  </si>
-  <si>
-    <t>Federal Reserve Economic Data, Federal Reserve Bank of St. Louis</t>
-  </si>
-  <si>
-    <t>Link: https://fred.stlouisfed.org</t>
-  </si>
-  <si>
-    <t>Help: https://fredhelp.stlouisfed.org</t>
-  </si>
-  <si>
-    <t>This data may be copyrighted. Please refer to the Terms of Use: https://fred.stlouisfed.org/legal#fred-terms-faq</t>
-  </si>
-  <si>
-    <t>File Created: 2025-11-18 7:55 am CST</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>UNRATE</t>
-  </si>
-  <si>
-    <t>Unemployment Rate, Percent, Monthly, Seasonally Adjusted</t>
-  </si>
-  <si>
-    <t>Data Updated: 2025-09-05</t>
   </si>
   <si>
     <t>date</t>
@@ -113,11 +88,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -426,65 +398,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="85.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B122"/>
   <sheetViews>
@@ -495,982 +408,982 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>42005</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>5.7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>42036</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>42064</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>42095</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>5.4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>42125</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>5.6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>42156</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>42186</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>42217</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>42248</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>42278</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>42309</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>42339</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>42370</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4.8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>42401</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>42430</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>42461</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>42491</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>4.8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>42522</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>42552</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>4.8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>42583</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>42614</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>42644</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>42675</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>4.7</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>42705</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>4.7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>42736</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>4.7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>42767</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>42795</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>42826</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>42856</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>42887</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4.3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>42917</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>4.3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>42948</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>42979</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>4.3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>43009</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>43040</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>43070</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>43101</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>43132</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>43160</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>43191</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>43221</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>43252</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>43282</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>43313</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>43344</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>43374</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>43405</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>43435</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>43466</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>43497</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>43525</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>43556</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>43586</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>43617</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>43647</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>43678</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>43709</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>43739</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>43770</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>43800</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>43831</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>43862</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>43891</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>43922</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>14.8</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>43952</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>13.2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>43983</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>44013</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>10.199999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>44044</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>8.4</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>44075</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>7.8</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>44105</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>6.9</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>44136</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>6.7</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>44166</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>6.7</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>44197</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>6.4</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="4">
+      <c r="A75" s="3">
         <v>44228</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>6.2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>44256</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>6.1</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="4">
+      <c r="A77" s="3">
         <v>44287</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>6.1</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>44317</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>5.8</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="4">
+      <c r="A79" s="3">
         <v>44348</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>5.9</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>44378</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>5.4</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="4">
+      <c r="A81" s="3">
         <v>44409</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>44440</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>4.7</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="4">
+      <c r="A83" s="3">
         <v>44470</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>44501</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="4">
+      <c r="A85" s="3">
         <v>44531</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>44562</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="4">
+      <c r="A87" s="3">
         <v>44593</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="4">
+      <c r="A88" s="3">
         <v>44621</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="4">
+      <c r="A89" s="3">
         <v>44652</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="4">
+      <c r="A90" s="3">
         <v>44682</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="4">
+      <c r="A91" s="3">
         <v>44713</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="4">
+      <c r="A92" s="3">
         <v>44743</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="4">
+      <c r="A93" s="3">
         <v>44774</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="4">
+      <c r="A94" s="3">
         <v>44805</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="4">
+      <c r="A95" s="3">
         <v>44835</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="4">
+      <c r="A96" s="3">
         <v>44866</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="4">
+      <c r="A97" s="3">
         <v>44896</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="4">
+      <c r="A98" s="3">
         <v>44927</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="4">
+      <c r="A99" s="3">
         <v>44958</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="4">
+      <c r="A100" s="3">
         <v>44986</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="4">
+      <c r="A101" s="3">
         <v>45017</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>3.4</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="4">
+      <c r="A102" s="3">
         <v>45047</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="4">
+      <c r="A103" s="3">
         <v>45078</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="1">
         <v>3.6</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="4">
+      <c r="A104" s="3">
         <v>45108</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="4">
+      <c r="A105" s="3">
         <v>45139</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="4">
+      <c r="A106" s="3">
         <v>45170</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="4">
+      <c r="A107" s="3">
         <v>45200</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="4">
+      <c r="A108" s="3">
         <v>45231</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="4">
+      <c r="A109" s="3">
         <v>45261</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="1">
         <v>3.8</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="4">
+      <c r="A110" s="3">
         <v>45292</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="1">
         <v>3.7</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="4">
+      <c r="A111" s="3">
         <v>45323</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="4">
+      <c r="A112" s="3">
         <v>45352</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="4">
+      <c r="A113" s="3">
         <v>45383</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="1">
         <v>3.9</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="4">
+      <c r="A114" s="3">
         <v>45413</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="4">
+      <c r="A115" s="3">
         <v>45444</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="4">
+      <c r="A116" s="3">
         <v>45474</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="4">
+      <c r="A117" s="3">
         <v>45505</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="4">
+      <c r="A118" s="3">
         <v>45536</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="4">
+      <c r="A119" s="3">
         <v>45566</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="4">
+      <c r="A120" s="3">
         <v>45597</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="1">
         <v>4.2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="4">
+      <c r="A121" s="3">
         <v>45627</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4">
+      <c r="A122" s="3">
         <v>45658</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>